<commit_message>
Se agrega el manejo las hojas Terceros-Clientes-Validador y manejo de vendedores-códigos
</commit_message>
<xml_diff>
--- a/resources/users/users.xlsx
+++ b/resources/users/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>CodigoVendedor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>FechaModificacion</t>
         </is>
       </c>
@@ -463,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>gAAAAABnt48QO154F-38JX2GAOqq4QxivGaXaLI6JEJK2xyYmuZONqdLpcuxspVLaORJaeGaTsnyep7AqP4TOT83Jz6aQfHVIQ==</t>
+          <t>gAAAAABnt587EQgIJ1MPMEoc-hBYkmIEyHuyNhxhZKIlMkggewm5uRtSuHG9gpcixYu7gRNw5iEmCzwLgDTBV48lrxC7bWVEAg==</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +478,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-02-20 15:22:40</t>
+          <t>B024</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-02-20 16:31:39</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Versión 1.1.0: integración de diálogos, login, nuevo menú y mejoras en la interfaz
</commit_message>
<xml_diff>
--- a/resources/users/users.xlsx
+++ b/resources/users/users.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>gAAAAABnt587EQgIJ1MPMEoc-hBYkmIEyHuyNhxhZKIlMkggewm5uRtSuHG9gpcixYu7gRNw5iEmCzwLgDTBV48lrxC7bWVEAg==</t>
+          <t>gAAAAABnuKssvaBQSK08o25PCgSu998enZt_mR1cyCxR_-cvEXQJ7lIUZ87yG-tHHsOo3EF8Fak32eV-30hG9SEDHIbnEUayEg==</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -483,7 +483,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-02-20 16:31:39</t>
+          <t>2025-02-21 11:34:52</t>
         </is>
       </c>
     </row>

</xml_diff>